<commit_message>
[Modified] : Modified Pomodoro.xlsx in Pomodoro folder
</commit_message>
<xml_diff>
--- a/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/Pomodoro/Pomodoro.xlsx
+++ b/ToDoApp-Doc/Document/Diagram/Thiết Kế Phần Mềm/Thiết Kế Xử Lý/Pomodoro/Pomodoro.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dell\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{42987CE0-BBA4-4E43-A47C-C8CAE4ACE184}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD530CCA-075B-4450-8CC7-749D39010583}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11310" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="72">
   <si>
     <t>DANH SÁCH CÁC KIỂU DỮ LIỆU XỬ LÝ</t>
   </si>
@@ -87,16 +87,10 @@
     <t>string</t>
   </si>
   <si>
-    <t>varchar</t>
-  </si>
-  <si>
     <t>Lưu trữ chu kỳ thời gian sử dụng Pomodoro</t>
   </si>
   <si>
     <t>datetime</t>
-  </si>
-  <si>
-    <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU VARCHAR</t>
   </si>
   <si>
     <t>pomodoro_id</t>
@@ -135,12 +129,6 @@
     <t>&gt; 0</t>
   </si>
   <si>
-    <t>Tham chiếu tới task_id của bảng Task</t>
-  </si>
-  <si>
-    <t>7 kí tự</t>
-  </si>
-  <si>
     <t>Lưu trữ id của pomodoro và id của task</t>
   </si>
   <si>
@@ -148,9 +136,6 @@
   </si>
   <si>
     <t>True, false</t>
-  </si>
-  <si>
-    <t>Phải là duy nhất</t>
   </si>
   <si>
     <t>PD00001</t>
@@ -249,6 +234,15 @@
   <si>
     <t>Tự động thay đổi trạng thái task</t>
   </si>
+  <si>
+    <t>DANH SÁCH CÁC THUỘC TÍNH KIỂU DỮ LIỆU STRING</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Phải là duy nhất </t>
+  </si>
+  <si>
+    <t>Tham chiếu tới task_id của class Task</t>
+  </si>
 </sst>
 </file>
 
@@ -300,7 +294,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -360,11 +354,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -373,6 +378,7 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -396,9 +402,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -445,6 +448,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -732,8 +738,8 @@
   </sheetPr>
   <dimension ref="A1:AF1001"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
-      <selection activeCell="Y6" sqref="Y6"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L6" sqref="L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -750,7 +756,7 @@
     <col min="15" max="19" width="14.42578125" style="2"/>
     <col min="20" max="20" width="25" style="2" customWidth="1"/>
     <col min="21" max="21" width="14.42578125" style="2"/>
-    <col min="22" max="22" width="20.42578125" style="2" customWidth="1"/>
+    <col min="22" max="22" width="22.140625" style="2" customWidth="1"/>
     <col min="23" max="23" width="21.85546875" style="2" customWidth="1"/>
     <col min="24" max="26" width="14.42578125" style="2"/>
     <col min="27" max="27" width="15.5703125" style="2" customWidth="1"/>
@@ -760,79 +766,79 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9"/>
-      <c r="C1" s="9"/>
-      <c r="D1" s="9"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
       <c r="E1" s="1"/>
-      <c r="F1" s="15" t="s">
-        <v>23</v>
+      <c r="F1" s="16" t="s">
+        <v>69</v>
       </c>
-      <c r="G1" s="15"/>
-      <c r="H1" s="15"/>
-      <c r="I1" s="15"/>
-      <c r="J1" s="15"/>
-      <c r="K1" s="15"/>
+      <c r="G1" s="16"/>
+      <c r="H1" s="16"/>
+      <c r="I1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="K1" s="16"/>
       <c r="L1" s="1"/>
-      <c r="M1" s="6" t="s">
+      <c r="M1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="9"/>
-      <c r="O1" s="9"/>
-      <c r="P1" s="9"/>
-      <c r="Q1" s="9"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
       <c r="R1" s="1"/>
-      <c r="S1" s="6" t="s">
+      <c r="S1" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="T1" s="7"/>
-      <c r="U1" s="7"/>
-      <c r="V1" s="7"/>
-      <c r="W1" s="7"/>
-      <c r="X1" s="7"/>
+      <c r="T1" s="8"/>
+      <c r="U1" s="8"/>
+      <c r="V1" s="8"/>
+      <c r="W1" s="8"/>
+      <c r="X1" s="8"/>
       <c r="Y1" s="1"/>
-      <c r="Z1" s="8" t="s">
+      <c r="Z1" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
+      <c r="AA1" s="9"/>
+      <c r="AB1" s="9"/>
+      <c r="AC1" s="9"/>
+      <c r="AD1" s="9"/>
+      <c r="AE1" s="9"/>
+      <c r="AF1" s="9"/>
     </row>
     <row r="2" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="10" t="s">
+      <c r="B2" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="E2" s="1"/>
-      <c r="F2" s="10" t="s">
+      <c r="F2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="G2" s="10" t="s">
+      <c r="G2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="H2" s="10" t="s">
+      <c r="H2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="I2" s="10" t="s">
+      <c r="I2" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="J2" s="10" t="s">
+      <c r="J2" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="18" t="s">
         <v>7</v>
       </c>
       <c r="L2" s="1"/>
@@ -840,7 +846,7 @@
         <v>4</v>
       </c>
       <c r="N2" s="18" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="O2" s="18" t="s">
         <v>9</v>
@@ -852,22 +858,22 @@
         <v>7</v>
       </c>
       <c r="R2" s="1"/>
-      <c r="S2" s="10" t="s">
+      <c r="S2" s="11" t="s">
         <v>4</v>
       </c>
-      <c r="T2" s="10" t="s">
+      <c r="T2" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="V2" s="10" t="s">
+      <c r="V2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="W2" s="10" t="s">
+      <c r="W2" s="11" t="s">
         <v>6</v>
       </c>
-      <c r="X2" s="10" t="s">
+      <c r="X2" s="11" t="s">
         <v>7</v>
       </c>
       <c r="Y2" s="29"/>
@@ -898,109 +904,107 @@
         <v>1</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C3" s="23" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
       <c r="D3" s="4"/>
       <c r="E3" s="1"/>
-      <c r="F3" s="11">
+      <c r="F3" s="12">
         <v>1</v>
       </c>
-      <c r="G3" s="11" t="s">
-        <v>24</v>
+      <c r="G3" s="12" t="s">
+        <v>22</v>
       </c>
-      <c r="H3" s="11" t="s">
-        <v>20</v>
+      <c r="H3" s="12" t="s">
+        <v>19</v>
       </c>
-      <c r="I3" s="11" t="s">
+      <c r="I3" s="12" t="s">
+        <v>70</v>
+      </c>
+      <c r="J3" s="34" t="s">
         <v>37</v>
       </c>
-      <c r="J3" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="K3" s="16" t="s">
-        <v>41</v>
-      </c>
+      <c r="K3" s="6"/>
       <c r="L3" s="1"/>
-      <c r="M3" s="14">
+      <c r="M3" s="15">
         <v>1</v>
       </c>
-      <c r="N3" s="14" t="s">
+      <c r="N3" s="15" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="15" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="O3" s="14" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="Q3" s="14"/>
+      <c r="Q3" s="15"/>
       <c r="R3" s="1"/>
       <c r="S3" s="23">
         <v>1</v>
       </c>
       <c r="T3" s="23" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="U3" s="23" t="s">
         <v>19</v>
       </c>
       <c r="V3" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="W3" s="23" t="s">
         <v>51</v>
       </c>
-      <c r="W3" s="23" t="s">
-        <v>56</v>
-      </c>
       <c r="X3" s="23" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="Y3" s="29"/>
-      <c r="Z3" s="14">
+      <c r="Z3" s="15">
         <v>1</v>
       </c>
       <c r="AA3" s="30" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="AB3" s="30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="AC3" s="30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AD3" s="30"/>
       <c r="AE3" s="26" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="AF3" s="30"/>
     </row>
     <row r="4" spans="1:32" ht="56.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="11">
+      <c r="A4" s="12">
         <v>2</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="12" t="s">
         <v>18</v>
       </c>
       <c r="C4" s="24" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
-      <c r="D4" s="12"/>
+      <c r="D4" s="13"/>
       <c r="E4" s="1"/>
-      <c r="F4" s="14">
+      <c r="F4" s="15">
         <v>2</v>
       </c>
-      <c r="G4" s="14" t="s">
-        <v>25</v>
+      <c r="G4" s="15" t="s">
+        <v>23</v>
       </c>
-      <c r="H4" s="14" t="s">
-        <v>20</v>
+      <c r="H4" s="15" t="s">
+        <v>19</v>
       </c>
       <c r="I4" s="19" t="s">
-        <v>36</v>
+        <v>71</v>
       </c>
-      <c r="J4" s="14" t="s">
-        <v>62</v>
+      <c r="J4" s="15" t="s">
+        <v>57</v>
       </c>
       <c r="K4" s="17"/>
       <c r="L4" s="1"/>
@@ -1014,16 +1018,16 @@
         <v>2</v>
       </c>
       <c r="T4" s="23" t="s">
-        <v>47</v>
+        <v>42</v>
       </c>
       <c r="U4" s="23" t="s">
         <v>19</v>
       </c>
       <c r="V4" s="23" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="W4" s="23" t="s">
-        <v>57</v>
+        <v>52</v>
       </c>
       <c r="X4" s="3"/>
       <c r="Y4" s="29"/>
@@ -1031,29 +1035,29 @@
         <v>2</v>
       </c>
       <c r="AA4" s="30" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="AB4" s="30" t="s">
-        <v>70</v>
+        <v>65</v>
       </c>
       <c r="AC4" s="30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AD4" s="30"/>
       <c r="AE4" s="26" t="s">
-        <v>71</v>
+        <v>66</v>
       </c>
       <c r="AF4" s="30"/>
     </row>
     <row r="5" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="14">
+      <c r="A5" s="15">
         <v>3</v>
       </c>
-      <c r="B5" s="14" t="s">
-        <v>66</v>
+      <c r="B5" s="15" t="s">
+        <v>61</v>
       </c>
       <c r="C5" s="19" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="1"/>
@@ -1074,57 +1078,57 @@
         <v>3</v>
       </c>
       <c r="T5" s="23" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="U5" s="23" t="s">
         <v>19</v>
       </c>
       <c r="V5" s="23" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
       <c r="W5" s="23" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="X5" s="3"/>
       <c r="Y5" s="29"/>
-      <c r="Z5" s="14">
+      <c r="Z5" s="15">
         <v>3</v>
       </c>
       <c r="AA5" s="30" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="AB5" s="30" t="s">
-        <v>44</v>
+        <v>39</v>
       </c>
       <c r="AC5" s="30" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="AD5" s="30"/>
       <c r="AE5" s="26" t="s">
-        <v>65</v>
+        <v>60</v>
       </c>
       <c r="AF5" s="30"/>
     </row>
     <row r="6" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="14">
+      <c r="A6" s="15">
         <v>4</v>
       </c>
-      <c r="B6" s="14" t="s">
-        <v>67</v>
+      <c r="B6" s="15" t="s">
+        <v>62</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>69</v>
+        <v>64</v>
       </c>
-      <c r="D6" s="14"/>
+      <c r="D6" s="15"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="15" t="s">
-        <v>26</v>
+      <c r="F6" s="16" t="s">
+        <v>24</v>
       </c>
-      <c r="G6" s="15"/>
-      <c r="H6" s="15"/>
-      <c r="I6" s="15"/>
-      <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="G6" s="16"/>
+      <c r="H6" s="16"/>
+      <c r="I6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="K6" s="16"/>
       <c r="L6" s="1"/>
       <c r="M6" s="20"/>
       <c r="N6" s="20"/>
@@ -1136,20 +1140,20 @@
         <v>4</v>
       </c>
       <c r="T6" s="3" t="s">
-        <v>49</v>
+        <v>44</v>
       </c>
       <c r="U6" s="23" t="s">
         <v>19</v>
       </c>
       <c r="V6" s="23" t="s">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="W6" s="23" t="s">
-        <v>59</v>
+        <v>54</v>
       </c>
       <c r="X6" s="3"/>
       <c r="Y6" s="29"/>
-      <c r="Z6" s="13"/>
+      <c r="Z6" s="14"/>
       <c r="AA6" s="33"/>
       <c r="AB6" s="33"/>
       <c r="AC6" s="33"/>
@@ -1158,10 +1162,10 @@
       <c r="AF6" s="33"/>
     </row>
     <row r="7" spans="1:32" ht="51.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="13"/>
-      <c r="B7" s="13"/>
+      <c r="A7" s="14"/>
+      <c r="B7" s="14"/>
       <c r="C7" s="25"/>
-      <c r="D7" s="13"/>
+      <c r="D7" s="14"/>
       <c r="E7" s="1"/>
       <c r="F7" s="18" t="s">
         <v>4</v>
@@ -1188,24 +1192,24 @@
       <c r="P7" s="20"/>
       <c r="Q7" s="20"/>
       <c r="R7" s="1"/>
-      <c r="S7" s="11">
+      <c r="S7" s="12">
         <v>5</v>
       </c>
-      <c r="T7" s="11" t="s">
-        <v>50</v>
+      <c r="T7" s="12" t="s">
+        <v>45</v>
       </c>
       <c r="U7" s="24" t="s">
         <v>19</v>
       </c>
       <c r="V7" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="W7" s="24" t="s">
         <v>55</v>
       </c>
-      <c r="W7" s="24" t="s">
-        <v>60</v>
-      </c>
-      <c r="X7" s="11"/>
+      <c r="X7" s="12"/>
       <c r="Y7" s="29"/>
-      <c r="Z7" s="13"/>
+      <c r="Z7" s="14"/>
       <c r="AA7" s="33"/>
       <c r="AB7" s="33"/>
       <c r="AC7" s="33"/>
@@ -1214,27 +1218,27 @@
       <c r="AF7" s="33"/>
     </row>
     <row r="8" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="13"/>
-      <c r="B8" s="13"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="13"/>
+      <c r="A8" s="14"/>
+      <c r="B8" s="14"/>
+      <c r="C8" s="14"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="14">
+      <c r="F8" s="15">
         <v>1</v>
       </c>
       <c r="G8" s="19" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I8" s="14" t="s">
-        <v>35</v>
+      <c r="I8" s="15" t="s">
+        <v>33</v>
       </c>
-      <c r="J8" s="14">
+      <c r="J8" s="15">
         <v>0</v>
       </c>
-      <c r="K8" s="14"/>
+      <c r="K8" s="15"/>
       <c r="L8" s="1"/>
       <c r="M8" s="20"/>
       <c r="N8" s="20"/>
@@ -1242,24 +1246,24 @@
       <c r="P8" s="20"/>
       <c r="Q8" s="20"/>
       <c r="R8" s="1"/>
-      <c r="S8" s="14">
+      <c r="S8" s="15">
         <v>6</v>
       </c>
-      <c r="T8" s="14" t="s">
-        <v>61</v>
+      <c r="T8" s="15" t="s">
+        <v>56</v>
       </c>
-      <c r="U8" s="14" t="s">
+      <c r="U8" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="V8" s="14">
+      <c r="V8" s="15">
         <v>0</v>
       </c>
       <c r="W8" s="19" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
-      <c r="X8" s="14"/>
+      <c r="X8" s="15"/>
       <c r="Y8" s="29"/>
-      <c r="Z8" s="13"/>
+      <c r="Z8" s="14"/>
       <c r="AA8" s="33"/>
       <c r="AB8" s="33"/>
       <c r="AC8" s="33"/>
@@ -1268,10 +1272,10 @@
       <c r="AF8" s="33"/>
     </row>
     <row r="9" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="13"/>
-      <c r="B9" s="13"/>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
+      <c r="A9" s="14"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="14"/>
+      <c r="D9" s="14"/>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
@@ -1286,14 +1290,14 @@
       <c r="P9" s="20"/>
       <c r="Q9" s="20"/>
       <c r="R9" s="1"/>
-      <c r="S9" s="13"/>
-      <c r="T9" s="13"/>
-      <c r="U9" s="13"/>
-      <c r="V9" s="13"/>
-      <c r="W9" s="13"/>
-      <c r="X9" s="13"/>
+      <c r="S9" s="14"/>
+      <c r="T9" s="14"/>
+      <c r="U9" s="14"/>
+      <c r="V9" s="14"/>
+      <c r="W9" s="14"/>
+      <c r="X9" s="14"/>
       <c r="Y9" s="29"/>
-      <c r="Z9" s="13"/>
+      <c r="Z9" s="14"/>
       <c r="AA9" s="33"/>
       <c r="AB9" s="33"/>
       <c r="AC9" s="33"/>
@@ -1302,13 +1306,13 @@
       <c r="AF9" s="33"/>
     </row>
     <row r="10" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="13"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
+      <c r="A10" s="14"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="14"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="1"/>
       <c r="F10" s="21" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="G10" s="21"/>
       <c r="H10" s="21"/>
@@ -1322,14 +1326,14 @@
       <c r="P10" s="20"/>
       <c r="Q10" s="20"/>
       <c r="R10" s="1"/>
-      <c r="S10" s="13"/>
-      <c r="T10" s="13"/>
-      <c r="U10" s="13"/>
-      <c r="V10" s="13"/>
-      <c r="W10" s="13"/>
-      <c r="X10" s="13"/>
+      <c r="S10" s="14"/>
+      <c r="T10" s="14"/>
+      <c r="U10" s="14"/>
+      <c r="V10" s="14"/>
+      <c r="W10" s="14"/>
+      <c r="X10" s="14"/>
       <c r="Y10" s="29"/>
-      <c r="Z10" s="13"/>
+      <c r="Z10" s="14"/>
       <c r="AA10" s="33"/>
       <c r="AB10" s="33"/>
       <c r="AC10" s="33"/>
@@ -1338,10 +1342,10 @@
       <c r="AF10" s="33"/>
     </row>
     <row r="11" spans="1:32" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="13"/>
-      <c r="B11" s="13"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="13"/>
+      <c r="A11" s="14"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="14"/>
+      <c r="D11" s="14"/>
       <c r="E11" s="1"/>
       <c r="F11" s="22" t="s">
         <v>4</v>
@@ -1368,14 +1372,14 @@
       <c r="P11" s="20"/>
       <c r="Q11" s="20"/>
       <c r="R11" s="1"/>
-      <c r="S11" s="13"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="13"/>
-      <c r="X11" s="13"/>
+      <c r="S11" s="14"/>
+      <c r="T11" s="14"/>
+      <c r="U11" s="14"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="14"/>
       <c r="Y11" s="29"/>
-      <c r="Z11" s="13"/>
+      <c r="Z11" s="14"/>
       <c r="AA11" s="33"/>
       <c r="AB11" s="33"/>
       <c r="AC11" s="33"/>
@@ -1384,27 +1388,27 @@
       <c r="AF11" s="33"/>
     </row>
     <row r="12" spans="1:32" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
+      <c r="A12" s="14"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="14"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="1"/>
-      <c r="F12" s="14">
+      <c r="F12" s="15">
         <v>1</v>
       </c>
       <c r="G12" s="19" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
-      <c r="H12" s="14" t="s">
-        <v>22</v>
+      <c r="H12" s="15" t="s">
+        <v>21</v>
       </c>
       <c r="I12" s="19" t="s">
-        <v>72</v>
+        <v>67</v>
       </c>
-      <c r="J12" s="14" t="s">
-        <v>30</v>
+      <c r="J12" s="15" t="s">
+        <v>28</v>
       </c>
-      <c r="K12" s="14"/>
+      <c r="K12" s="15"/>
       <c r="L12" s="1"/>
       <c r="M12" s="20"/>
       <c r="N12" s="20"/>
@@ -1412,14 +1416,14 @@
       <c r="P12" s="20"/>
       <c r="Q12" s="20"/>
       <c r="R12" s="1"/>
-      <c r="S12" s="13"/>
-      <c r="T12" s="13"/>
-      <c r="U12" s="13"/>
-      <c r="V12" s="13"/>
-      <c r="W12" s="13"/>
-      <c r="X12" s="13"/>
+      <c r="S12" s="14"/>
+      <c r="T12" s="14"/>
+      <c r="U12" s="14"/>
+      <c r="V12" s="14"/>
+      <c r="W12" s="14"/>
+      <c r="X12" s="14"/>
       <c r="Y12" s="29"/>
-      <c r="Z12" s="13"/>
+      <c r="Z12" s="14"/>
       <c r="AA12" s="33"/>
       <c r="AB12" s="33"/>
       <c r="AC12" s="33"/>
@@ -1428,7 +1432,7 @@
       <c r="AF12" s="33"/>
     </row>
     <row r="13" spans="1:32" ht="50.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="13"/>
+      <c r="A13" s="14"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
@@ -1446,14 +1450,14 @@
       <c r="P13" s="20"/>
       <c r="Q13" s="20"/>
       <c r="R13" s="1"/>
-      <c r="S13" s="13"/>
-      <c r="T13" s="13"/>
-      <c r="U13" s="13"/>
-      <c r="V13" s="13"/>
-      <c r="W13" s="13"/>
-      <c r="X13" s="13"/>
+      <c r="S13" s="14"/>
+      <c r="T13" s="14"/>
+      <c r="U13" s="14"/>
+      <c r="V13" s="14"/>
+      <c r="W13" s="14"/>
+      <c r="X13" s="14"/>
       <c r="Y13" s="29"/>
-      <c r="Z13" s="13"/>
+      <c r="Z13" s="14"/>
       <c r="AA13" s="33"/>
       <c r="AB13" s="33"/>
       <c r="AC13" s="33"/>
@@ -1480,14 +1484,14 @@
       <c r="P14" s="20"/>
       <c r="Q14" s="20"/>
       <c r="R14" s="1"/>
-      <c r="S14" s="13"/>
-      <c r="T14" s="13"/>
-      <c r="U14" s="13"/>
-      <c r="V14" s="13"/>
-      <c r="W14" s="13"/>
-      <c r="X14" s="13"/>
+      <c r="S14" s="14"/>
+      <c r="T14" s="14"/>
+      <c r="U14" s="14"/>
+      <c r="V14" s="14"/>
+      <c r="W14" s="14"/>
+      <c r="X14" s="14"/>
       <c r="Y14" s="29"/>
-      <c r="Z14" s="13"/>
+      <c r="Z14" s="14"/>
       <c r="AA14" s="33"/>
       <c r="AB14" s="33"/>
       <c r="AC14" s="33"/>
@@ -1514,14 +1518,14 @@
       <c r="P15" s="20"/>
       <c r="Q15" s="20"/>
       <c r="R15" s="1"/>
-      <c r="S15" s="13"/>
-      <c r="T15" s="13"/>
-      <c r="U15" s="13"/>
-      <c r="V15" s="13"/>
-      <c r="W15" s="13"/>
-      <c r="X15" s="13"/>
+      <c r="S15" s="14"/>
+      <c r="T15" s="14"/>
+      <c r="U15" s="14"/>
+      <c r="V15" s="14"/>
+      <c r="W15" s="14"/>
+      <c r="X15" s="14"/>
       <c r="Y15" s="29"/>
-      <c r="Z15" s="13"/>
+      <c r="Z15" s="14"/>
       <c r="AA15" s="33"/>
       <c r="AB15" s="33"/>
       <c r="AC15" s="33"/>
@@ -1548,14 +1552,14 @@
       <c r="P16" s="20"/>
       <c r="Q16" s="20"/>
       <c r="R16" s="1"/>
-      <c r="S16" s="13"/>
-      <c r="T16" s="13"/>
-      <c r="U16" s="13"/>
-      <c r="V16" s="13"/>
-      <c r="W16" s="13"/>
-      <c r="X16" s="13"/>
+      <c r="S16" s="14"/>
+      <c r="T16" s="14"/>
+      <c r="U16" s="14"/>
+      <c r="V16" s="14"/>
+      <c r="W16" s="14"/>
+      <c r="X16" s="14"/>
       <c r="Y16" s="29"/>
-      <c r="Z16" s="13"/>
+      <c r="Z16" s="14"/>
       <c r="AA16" s="33"/>
       <c r="AB16" s="33"/>
       <c r="AC16" s="33"/>
@@ -1582,14 +1586,14 @@
       <c r="P17" s="20"/>
       <c r="Q17" s="20"/>
       <c r="R17" s="1"/>
-      <c r="S17" s="13"/>
-      <c r="T17" s="13"/>
-      <c r="U17" s="13"/>
-      <c r="V17" s="13"/>
-      <c r="W17" s="13"/>
-      <c r="X17" s="13"/>
+      <c r="S17" s="14"/>
+      <c r="T17" s="14"/>
+      <c r="U17" s="14"/>
+      <c r="V17" s="14"/>
+      <c r="W17" s="14"/>
+      <c r="X17" s="14"/>
       <c r="Y17" s="29"/>
-      <c r="Z17" s="13"/>
+      <c r="Z17" s="14"/>
       <c r="AA17" s="33"/>
       <c r="AB17" s="33"/>
       <c r="AC17" s="33"/>
@@ -1616,14 +1620,14 @@
       <c r="P18" s="20"/>
       <c r="Q18" s="20"/>
       <c r="R18" s="1"/>
-      <c r="S18" s="13"/>
-      <c r="T18" s="13"/>
-      <c r="U18" s="13"/>
-      <c r="V18" s="13"/>
-      <c r="W18" s="13"/>
-      <c r="X18" s="13"/>
+      <c r="S18" s="14"/>
+      <c r="T18" s="14"/>
+      <c r="U18" s="14"/>
+      <c r="V18" s="14"/>
+      <c r="W18" s="14"/>
+      <c r="X18" s="14"/>
       <c r="Y18" s="29"/>
-      <c r="Z18" s="13"/>
+      <c r="Z18" s="14"/>
       <c r="AA18" s="33"/>
       <c r="AB18" s="33"/>
       <c r="AC18" s="33"/>
@@ -1650,14 +1654,14 @@
       <c r="P19" s="20"/>
       <c r="Q19" s="20"/>
       <c r="R19" s="1"/>
-      <c r="S19" s="13"/>
-      <c r="T19" s="13"/>
-      <c r="U19" s="13"/>
-      <c r="V19" s="13"/>
-      <c r="W19" s="13"/>
-      <c r="X19" s="13"/>
+      <c r="S19" s="14"/>
+      <c r="T19" s="14"/>
+      <c r="U19" s="14"/>
+      <c r="V19" s="14"/>
+      <c r="W19" s="14"/>
+      <c r="X19" s="14"/>
       <c r="Y19" s="29"/>
-      <c r="Z19" s="13"/>
+      <c r="Z19" s="14"/>
       <c r="AA19" s="33"/>
       <c r="AB19" s="33"/>
       <c r="AC19" s="33"/>
@@ -1684,14 +1688,14 @@
       <c r="P20" s="20"/>
       <c r="Q20" s="20"/>
       <c r="R20" s="1"/>
-      <c r="S20" s="13"/>
-      <c r="T20" s="13"/>
-      <c r="U20" s="13"/>
-      <c r="V20" s="13"/>
-      <c r="W20" s="13"/>
-      <c r="X20" s="13"/>
+      <c r="S20" s="14"/>
+      <c r="T20" s="14"/>
+      <c r="U20" s="14"/>
+      <c r="V20" s="14"/>
+      <c r="W20" s="14"/>
+      <c r="X20" s="14"/>
       <c r="Y20" s="29"/>
-      <c r="Z20" s="13"/>
+      <c r="Z20" s="14"/>
       <c r="AA20" s="33"/>
       <c r="AB20" s="33"/>
       <c r="AC20" s="33"/>
@@ -1725,7 +1729,7 @@
       <c r="W21" s="29"/>
       <c r="X21" s="29"/>
       <c r="Y21" s="29"/>
-      <c r="Z21" s="13"/>
+      <c r="Z21" s="14"/>
       <c r="AA21" s="33"/>
       <c r="AB21" s="33"/>
       <c r="AC21" s="33"/>
@@ -1759,7 +1763,7 @@
       <c r="W22" s="29"/>
       <c r="X22" s="29"/>
       <c r="Y22" s="29"/>
-      <c r="Z22" s="13"/>
+      <c r="Z22" s="14"/>
       <c r="AA22" s="33"/>
       <c r="AB22" s="33"/>
       <c r="AC22" s="33"/>
@@ -1793,7 +1797,7 @@
       <c r="W23" s="29"/>
       <c r="X23" s="29"/>
       <c r="Y23" s="29"/>
-      <c r="Z23" s="13"/>
+      <c r="Z23" s="14"/>
       <c r="AA23" s="33"/>
       <c r="AB23" s="33"/>
       <c r="AC23" s="33"/>

</xml_diff>